<commit_message>
feat: add new usb datasheet
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -474,25 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -503,6 +485,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,7 +1350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1360,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1379,52 +1379,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1434,146 +1434,146 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="9"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="11" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="16"/>
-      <c r="B5" s="15">
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="11"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="16"/>
-      <c r="B6" s="15">
+      <c r="B6" s="10">
         <v>3</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="11"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="16"/>
-      <c r="B7" s="15">
+      <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="11"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="16"/>
-      <c r="B8" s="15">
+      <c r="B8" s="10">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="11"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="16"/>
-      <c r="B9" s="15">
+      <c r="B9" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
         <v>0</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5">
@@ -1595,19 +1595,19 @@
       <c r="I10" s="5">
         <v>3.6</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="9"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1616,10 +1616,10 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="9"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1633,10 +1633,10 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="9"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -1653,11 +1653,11 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="14"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="9"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1677,10 +1677,10 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="9"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -1697,17 +1697,17 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="9"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1722,10 +1722,10 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="9"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1745,10 +1745,10 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5">
@@ -1757,7 +1757,7 @@
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1769,19 +1769,19 @@
       <c r="I18" s="5">
         <v>5</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="18" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="9"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1790,10 +1790,10 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="9"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
@@ -1811,10 +1811,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="9"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
@@ -1832,10 +1832,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="11"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="9"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -1853,10 +1853,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="11"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="9"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -1874,10 +1874,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="9"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -1895,10 +1895,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="11"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="9"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
@@ -1916,10 +1916,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="11"/>
+      <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="9"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
@@ -1940,10 +1940,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="11"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="9"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
@@ -1964,10 +1964,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="11"/>
+      <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="9"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
@@ -1988,10 +1988,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="11"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="9"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
@@ -2012,10 +2012,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="11"/>
+      <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="9"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
@@ -2036,10 +2036,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="11"/>
+      <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="9"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
@@ -2060,10 +2060,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="11"/>
+      <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="9"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
@@ -2084,10 +2084,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="11"/>
+      <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="9"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
@@ -2108,10 +2108,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="11"/>
+      <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="9"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2132,10 +2132,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="11"/>
+      <c r="J34" s="17"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="9"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
@@ -2153,10 +2153,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="11"/>
+      <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="5">
@@ -2165,7 +2165,7 @@
       <c r="C36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="8" t="s">
@@ -2178,14 +2178,14 @@
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="10"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="5">
         <v>2</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="11" t="s">
         <v>89</v>
       </c>
       <c r="E37" s="8" t="s">
@@ -2198,7 +2198,7 @@
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="10"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="5">
         <v>3</v>
       </c>
@@ -2218,7 +2218,7 @@
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="10"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="5">
         <v>4</v>
       </c>
@@ -2238,7 +2238,7 @@
       </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="9"/>
+      <c r="A41" s="14"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="9"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="9"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
@@ -2291,31 +2291,31 @@
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="9"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="9"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="9"/>
+      <c r="A46" s="14"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
@@ -2327,7 +2327,7 @@
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="9"/>
+      <c r="A47" s="14"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="9"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2352,7 +2352,7 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="9"/>
+      <c r="A49" s="14"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="9"/>
+      <c r="A50" s="14"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="9"/>
+      <c r="A51" s="14"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2383,7 +2383,7 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="9"/>
+      <c r="A52" s="14"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2392,7 +2392,7 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="9"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="9"/>
+      <c r="A54" s="14"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2412,7 +2412,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="9"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2421,55 +2421,55 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="9"/>
+      <c r="A56" s="14"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="9"/>
+      <c r="A57" s="14"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="18" t="s">
+      <c r="D57" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="9"/>
+      <c r="A58" s="14"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="9"/>
+      <c r="A59" s="14"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="9"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2478,7 +2478,7 @@
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="9"/>
+      <c r="A61" s="14"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2487,7 +2487,7 @@
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="9"/>
+      <c r="A62" s="14"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2496,7 +2496,7 @@
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="9"/>
+      <c r="A63" s="14"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2505,7 +2505,7 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="9"/>
+      <c r="A64" s="14"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2514,7 +2514,7 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="9"/>
+      <c r="A65" s="14"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2523,31 +2523,31 @@
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="9"/>
+      <c r="A66" s="14"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D66" s="17" t="s">
+      <c r="D66" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="9"/>
+      <c r="A67" s="14"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="9"/>
+      <c r="A68" s="14"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="9"/>
+      <c r="A69" s="14"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2569,7 +2569,7 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="9"/>
+      <c r="A70" s="14"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2582,7 +2582,7 @@
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="9"/>
+      <c r="A71" s="14"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2595,7 +2595,7 @@
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="9"/>
+      <c r="A72" s="14"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2608,7 +2608,7 @@
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="9"/>
+      <c r="A73" s="14"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2621,7 +2621,7 @@
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="9"/>
+      <c r="A74" s="14"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2634,7 +2634,7 @@
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="9"/>
+      <c r="A75" s="14"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2647,7 +2647,7 @@
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="9"/>
+      <c r="A76" s="14"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2660,31 +2660,31 @@
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="9"/>
+      <c r="A77" s="14"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="17" t="s">
+      <c r="D77" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="9"/>
+      <c r="A78" s="14"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D78" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="9"/>
+      <c r="A79" s="14"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
@@ -2693,7 +2693,7 @@
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="9"/>
+      <c r="A80" s="14"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="9"/>
+      <c r="A81" s="14"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2711,7 +2711,7 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="9"/>
+      <c r="A82" s="14"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2720,7 +2720,7 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="9"/>
+      <c r="A83" s="14"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2733,6 +2733,14 @@
     <sortCondition descending="1" ref="H44"/>
   </sortState>
   <mergeCells count="17">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A83"/>
     <mergeCell ref="J2:J3"/>
@@ -2742,14 +2750,6 @@
     <mergeCell ref="J10:J17"/>
     <mergeCell ref="A18:A35"/>
     <mergeCell ref="J18:J35"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2792,52 +2792,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2847,10 +2847,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="9"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -2865,12 +2865,12 @@
       <c r="H4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="9"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -2883,10 +2883,10 @@
       <c r="H5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="9"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -2899,10 +2899,10 @@
       <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="9"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -2915,10 +2915,10 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="9"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -2937,10 +2937,10 @@
       <c r="I8" s="1">
         <v>5.5</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="9"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -2953,10 +2953,10 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -2975,12 +2975,12 @@
       <c r="I10" s="1">
         <v>3.6</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="9"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -2993,10 +2993,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="9"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3010,10 +3010,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="9"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3030,11 +3030,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="14"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="9"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3051,10 +3051,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="9"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3071,10 +3071,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="9"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3093,10 +3093,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="9"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3113,10 +3113,10 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1">
@@ -3134,12 +3134,12 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="18" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="9"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3152,10 +3152,10 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="9"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3173,10 +3173,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="9"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3194,10 +3194,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="11"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="9"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3215,10 +3215,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="11"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="9"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3236,10 +3236,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="9"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3257,10 +3257,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="11"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="9"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3278,10 +3278,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="11"/>
+      <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="9"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3299,10 +3299,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="11"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="9"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3320,10 +3320,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="11"/>
+      <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="9"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3341,10 +3341,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="11"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="9"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3362,10 +3362,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="11"/>
+      <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="9"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3383,10 +3383,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="11"/>
+      <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="9"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3404,10 +3404,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="11"/>
+      <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="9"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3425,10 +3425,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="11"/>
+      <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="9"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3446,10 +3446,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="11"/>
+      <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="9"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3467,10 +3467,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="11"/>
+      <c r="J34" s="17"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="9"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3488,10 +3488,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="11"/>
+      <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="4">
@@ -3511,7 +3511,7 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="10"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="4">
         <v>2</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="10"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="4">
         <v>3</v>
       </c>
@@ -3547,7 +3547,7 @@
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="10"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="4">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
feat: add a test comment
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolentino\Documents\test\Kicad\Projects\CameraSystem\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10590" windowHeight="8670"/>
   </bookViews>
@@ -11,9 +16,9 @@
     <sheet name="Power Consumption" sheetId="3" r:id="rId2"/>
     <sheet name="Pinout_Old" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="118">
   <si>
     <t>Component</t>
   </si>
@@ -384,12 +389,15 @@
   <si>
     <t>CAM_D0</t>
   </si>
+  <si>
+    <t>test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,10 +495,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -506,7 +514,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1350,21 +1358,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1378,53 +1386,53 @@
     <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="14" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1434,9 +1442,9 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>104</v>
       </c>
@@ -1462,7 +1470,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="10">
         <v>2</v>
@@ -1484,7 +1492,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="10">
         <v>3</v>
@@ -1506,7 +1514,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="10">
         <v>4</v>
@@ -1528,7 +1536,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="10">
         <v>5</v>
@@ -1550,7 +1558,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="10">
         <v>6</v>
@@ -1572,8 +1580,8 @@
       <c r="I9" s="10"/>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5">
@@ -1595,12 +1603,12 @@
       <c r="I10" s="5">
         <v>3.6</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1616,10 +1624,10 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="14"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1633,10 +1641,10 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="14"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -1653,11 +1661,11 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="14"/>
+      <c r="J13" s="13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="14"/>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1677,10 +1685,10 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="14"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -1697,10 +1705,10 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="14"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1722,10 +1730,13 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="14"/>
+      <c r="J16" s="13"/>
+      <c r="Q16" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1745,10 +1756,10 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="13" t="s">
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5">
@@ -1773,8 +1784,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="14"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1792,8 +1803,8 @@
       </c>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
@@ -1813,8 +1824,8 @@
       </c>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="14"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
@@ -1834,8 +1845,8 @@
       </c>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="14"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -1855,8 +1866,8 @@
       </c>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="14"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -1876,8 +1887,8 @@
       </c>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="14"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -1897,8 +1908,8 @@
       </c>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="14"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
@@ -1918,8 +1929,8 @@
       </c>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="14"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
@@ -1942,8 +1953,8 @@
       </c>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="14"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
@@ -1966,8 +1977,8 @@
       </c>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="14"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
@@ -1990,8 +2001,8 @@
       </c>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="14"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
@@ -2014,8 +2025,8 @@
       </c>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="14"/>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
@@ -2038,8 +2049,8 @@
       </c>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="14"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
@@ -2062,8 +2073,8 @@
       </c>
       <c r="J31" s="17"/>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="14"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
@@ -2086,8 +2097,8 @@
       </c>
       <c r="J32" s="17"/>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="14"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
@@ -2110,8 +2121,8 @@
       </c>
       <c r="J33" s="17"/>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="14"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2134,8 +2145,8 @@
       </c>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="14"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
@@ -2155,8 +2166,8 @@
       </c>
       <c r="J35" s="17"/>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="5">
@@ -2177,8 +2188,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="13"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
       <c r="B37" s="5">
         <v>2</v>
       </c>
@@ -2197,8 +2208,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="13"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
       <c r="B38" s="5">
         <v>3</v>
       </c>
@@ -2217,8 +2228,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="13"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39" s="5">
         <v>4</v>
       </c>
@@ -2237,8 +2248,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="14" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2252,8 +2263,8 @@
         <v>SD_MISO</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="14"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2265,8 +2276,8 @@
         <v>SD_MOSI</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="14"/>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2278,8 +2289,8 @@
         <v>SD_SCK</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="14"/>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
@@ -2290,8 +2301,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="14"/>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
@@ -2302,8 +2313,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="14"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
@@ -2314,8 +2325,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="14"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
@@ -2326,8 +2337,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="14"/>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
@@ -2338,8 +2349,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="14"/>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2351,8 +2362,8 @@
         <v>WIFI_TX</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="14"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2364,8 +2375,8 @@
         <v>WIFI_RX</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="14"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2373,8 +2384,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="14"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2382,8 +2393,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="14"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2391,8 +2402,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="14"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -2401,8 +2412,8 @@
       </c>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="14"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2411,8 +2422,8 @@
       </c>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="14"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2420,8 +2431,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="14"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
@@ -2432,8 +2443,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="14"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
@@ -2444,8 +2455,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="14"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
@@ -2456,8 +2467,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="14"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
@@ -2468,8 +2479,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="14"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2477,8 +2488,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="14"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2486,8 +2497,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="14"/>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2495,8 +2506,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="14"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2504,8 +2515,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="14"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2513,8 +2524,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="14"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2522,8 +2533,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="14"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
@@ -2534,8 +2545,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="14"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
@@ -2546,8 +2557,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="14"/>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2555,8 +2566,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="14"/>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2568,8 +2579,8 @@
         <v>CAM_D7</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="14"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2581,8 +2592,8 @@
         <v>CAM_D6</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="14"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2594,8 +2605,8 @@
         <v>CAM_D5</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="14"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2607,8 +2618,8 @@
         <v>CAM_D4</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="14"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2620,8 +2631,8 @@
         <v>CAM_D3</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="14"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2633,8 +2644,8 @@
         <v>CAM_D2</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="14"/>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2646,8 +2657,8 @@
         <v>CAM_D1</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="14"/>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2659,8 +2670,8 @@
         <v>CAM_D0</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="14"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
@@ -2671,8 +2682,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="14"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
@@ -2683,8 +2694,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="14"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
@@ -2692,8 +2703,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="14"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
@@ -2701,8 +2712,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="14"/>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2710,8 +2721,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="14"/>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2719,8 +2730,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="14"/>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="13"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2733,14 +2744,6 @@
     <sortCondition descending="1" ref="H44"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I2"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A83"/>
     <mergeCell ref="J2:J3"/>
@@ -2750,6 +2753,14 @@
     <mergeCell ref="J10:J17"/>
     <mergeCell ref="A18:A35"/>
     <mergeCell ref="J18:J35"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2758,26 +2769,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2791,53 +2802,53 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="14" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2847,10 +2858,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="14" t="s">
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -2869,8 +2880,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="14"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -2885,8 +2896,8 @@
       </c>
       <c r="J5" s="17"/>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="14"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -2901,8 +2912,8 @@
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -2917,8 +2928,8 @@
       </c>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="14"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -2939,8 +2950,8 @@
       </c>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -2955,8 +2966,8 @@
       </c>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -2975,12 +2986,12 @@
       <c r="I10" s="1">
         <v>3.6</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -2993,10 +3004,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="14"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3010,10 +3021,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="14"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3030,11 +3041,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="14"/>
+      <c r="J13" s="13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="14"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3051,10 +3062,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="14"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3071,10 +3082,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="14"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3093,10 +3104,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="14"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3113,10 +3124,10 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="13" t="s">
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1">
@@ -3138,8 +3149,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="14"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3154,8 +3165,8 @@
       </c>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3175,8 +3186,8 @@
       </c>
       <c r="J20" s="17"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="14"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3196,8 +3207,8 @@
       </c>
       <c r="J21" s="17"/>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="14"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3217,8 +3228,8 @@
       </c>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="14"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3238,8 +3249,8 @@
       </c>
       <c r="J23" s="17"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="14"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3259,8 +3270,8 @@
       </c>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="14"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3280,8 +3291,8 @@
       </c>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="14"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3301,8 +3312,8 @@
       </c>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="14"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3322,8 +3333,8 @@
       </c>
       <c r="J27" s="17"/>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="14"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3343,8 +3354,8 @@
       </c>
       <c r="J28" s="17"/>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="14"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3364,8 +3375,8 @@
       </c>
       <c r="J29" s="17"/>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="14"/>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3385,8 +3396,8 @@
       </c>
       <c r="J30" s="17"/>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="14"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3406,8 +3417,8 @@
       </c>
       <c r="J31" s="17"/>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="14"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3427,8 +3438,8 @@
       </c>
       <c r="J32" s="17"/>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="14"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3448,8 +3459,8 @@
       </c>
       <c r="J33" s="17"/>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="14"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3469,8 +3480,8 @@
       </c>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="14"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3490,8 +3501,8 @@
       </c>
       <c r="J35" s="17"/>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="4">
@@ -3510,8 +3521,8 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="13"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
       <c r="B37" s="4">
         <v>2</v>
       </c>
@@ -3528,8 +3539,8 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="13"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
       <c r="B38" s="4">
         <v>3</v>
       </c>
@@ -3546,8 +3557,8 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="13"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39" s="4">
         <v>4</v>
       </c>
@@ -3564,7 +3575,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -3574,7 +3585,7 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>

</xml_diff>

<commit_message>
feat: add datasheet of oscillator and update pinout table
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="124">
   <si>
     <t>Component</t>
   </si>
@@ -391,6 +391,24 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Connected to peripheral component</t>
+  </si>
+  <si>
+    <t>Connected to another module (GPIO can change)</t>
+  </si>
+  <si>
+    <t>Connected to another module (GPIO cannot change)</t>
+  </si>
+  <si>
+    <t>LCD is connected to a  level shifter 3.3V</t>
+  </si>
+  <si>
+    <t>WIFI_EN</t>
   </si>
 </sst>
 </file>
@@ -406,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,8 +461,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -452,11 +488,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -498,7 +543,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -511,6 +562,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,16 +784,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533960</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>91888</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>600635</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>443753</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>72838</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -748,8 +811,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6496050" y="6781800"/>
-          <a:ext cx="2943225" cy="1123950"/>
+          <a:off x="9767607" y="6568888"/>
+          <a:ext cx="2935381" cy="1123950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1366,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:X83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,53 +1449,53 @@
     <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="13" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1442,10 +1505,10 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>104</v>
       </c>
       <c r="B4" s="10">
@@ -1466,12 +1529,12 @@
         <v>3.3</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
       <c r="B5" s="10">
         <v>2</v>
       </c>
@@ -1490,10 +1553,10 @@
         <v>3.3</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
       <c r="B6" s="10">
         <v>3</v>
       </c>
@@ -1512,10 +1575,10 @@
         <v>3.3</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
       <c r="B7" s="10">
         <v>4</v>
       </c>
@@ -1534,10 +1597,14 @@
         <v>3.3</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="J7" s="19"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
       <c r="B8" s="10">
         <v>5</v>
       </c>
@@ -1556,10 +1623,14 @@
         <v>3.3</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="J8" s="19"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
       <c r="B9" s="10">
         <v>6</v>
       </c>
@@ -1578,10 +1649,14 @@
         <v>0</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="J9" s="19"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5">
@@ -1590,7 +1665,7 @@
       <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -1603,12 +1678,20 @@
       <c r="I10" s="5">
         <v>3.6</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1624,15 +1707,25 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="J11" s="16"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="H12" s="5">
         <f>0.25*3.3</f>
@@ -1641,14 +1734,14 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="24" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1661,18 +1754,18 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="13"/>
+      <c r="J13" s="16"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -1685,14 +1778,14 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1705,10 +1798,10 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1730,20 +1823,20 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="13"/>
+      <c r="J16" s="16"/>
       <c r="Q16" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1756,10 +1849,10 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="13"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5">
@@ -1780,12 +1873,12 @@
       <c r="I18" s="5">
         <v>5</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1801,10 +1894,10 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="17"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
@@ -1822,10 +1915,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="17"/>
+      <c r="J20" s="19"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
@@ -1843,10 +1936,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="17"/>
+      <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -1864,10 +1957,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="17"/>
+      <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -1885,10 +1978,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="17"/>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -1906,10 +1999,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="17"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
@@ -1927,17 +2020,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="17"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1951,17 +2044,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="17"/>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -1975,17 +2068,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="17"/>
+      <c r="J27" s="19"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>111</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -1999,17 +2092,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="17"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -2023,17 +2116,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="17"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -2047,17 +2140,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="17"/>
+      <c r="J30" s="19"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -2071,17 +2164,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="17"/>
+      <c r="J31" s="19"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -2095,17 +2188,17 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="17"/>
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E33" s="5" t="s">
@@ -2119,10 +2212,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="17"/>
+      <c r="J33" s="19"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2143,10 +2236,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="17"/>
+      <c r="J34" s="19"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
@@ -2164,10 +2257,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="17"/>
+      <c r="J35" s="19"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="5">
@@ -2187,9 +2280,12 @@
       <c r="H36" s="8">
         <v>0</v>
       </c>
+      <c r="J36" s="16" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="5">
         <v>2</v>
       </c>
@@ -2207,16 +2303,17 @@
       <c r="H37" s="8">
         <v>5</v>
       </c>
+      <c r="J37" s="16"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="5">
         <v>3</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="22" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="8" t="s">
@@ -2227,16 +2324,17 @@
       <c r="H38" s="8">
         <v>5</v>
       </c>
+      <c r="J38" s="16"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="5">
         <v>4</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="22" t="s">
         <v>90</v>
       </c>
       <c r="E39" s="8" t="s">
@@ -2247,9 +2345,10 @@
       <c r="H39" s="8">
         <v>5</v>
       </c>
+      <c r="J39" s="16"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="16" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2264,7 +2363,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2277,7 +2376,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2290,7 +2389,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
@@ -2302,7 +2401,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
@@ -2314,7 +2413,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
@@ -2326,7 +2425,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
@@ -2338,7 +2437,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
@@ -2350,7 +2449,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2363,7 +2462,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2376,7 +2475,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2385,7 +2484,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2394,7 +2493,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2403,7 +2502,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -2413,7 +2512,7 @@
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2423,7 +2522,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2432,7 +2531,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
@@ -2444,7 +2543,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
@@ -2456,7 +2555,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
@@ -2468,7 +2567,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
@@ -2480,7 +2579,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2489,7 +2588,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2498,7 +2597,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2507,7 +2606,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2516,7 +2615,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
+      <c r="A64" s="16"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2525,7 +2624,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2534,7 +2633,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
@@ -2546,7 +2645,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
@@ -2558,7 +2657,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2567,7 +2666,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+      <c r="A69" s="16"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2580,7 +2679,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2593,7 +2692,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
+      <c r="A71" s="16"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2606,7 +2705,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
+      <c r="A72" s="16"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2619,7 +2718,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
+      <c r="A73" s="16"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2632,7 +2731,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2645,7 +2744,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
+      <c r="A75" s="16"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2658,7 +2757,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
+      <c r="A76" s="16"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2671,7 +2770,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
+      <c r="A77" s="16"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
@@ -2683,7 +2782,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
+      <c r="A78" s="16"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
@@ -2695,25 +2794,33 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
+      <c r="A79" s="16"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>102</v>
       </c>
+      <c r="D79" s="3" t="str">
+        <f>D12</f>
+        <v>WIFI_EN</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
+      <c r="A80" s="16"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>101</v>
       </c>
+      <c r="D80" s="3" t="str">
+        <f>D14</f>
+        <v>WIFI_RST</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
+      <c r="A81" s="16"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2722,7 +2829,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
+      <c r="A82" s="16"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2731,7 +2838,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
+      <c r="A83" s="16"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2743,7 +2850,15 @@
   <sortState ref="H44:I54">
     <sortCondition descending="1" ref="H44"/>
   </sortState>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A83"/>
     <mergeCell ref="J2:J3"/>
@@ -2753,14 +2868,7 @@
     <mergeCell ref="J10:J17"/>
     <mergeCell ref="A18:A35"/>
     <mergeCell ref="J18:J35"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J36:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2803,52 +2911,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="13" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2858,10 +2966,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -2876,12 +2984,12 @@
       <c r="H4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -2894,10 +3002,10 @@
       <c r="H5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="17"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -2910,10 +3018,10 @@
       <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="17"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -2926,10 +3034,10 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -2948,10 +3056,10 @@
       <c r="I8" s="1">
         <v>5.5</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -2964,10 +3072,10 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -2986,12 +3094,12 @@
       <c r="I10" s="1">
         <v>3.6</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -3004,10 +3112,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="13"/>
+      <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3021,10 +3129,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="13"/>
+      <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3041,11 +3149,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="13"/>
+      <c r="J13" s="16"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3062,10 +3170,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="13"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3082,10 +3190,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="13"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3104,10 +3212,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="13"/>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3124,10 +3232,10 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="13"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1">
@@ -3145,12 +3253,12 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3163,10 +3271,10 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="17"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3184,10 +3292,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="17"/>
+      <c r="J20" s="19"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3205,10 +3313,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="17"/>
+      <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3226,10 +3334,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="17"/>
+      <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3247,10 +3355,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="17"/>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3268,10 +3376,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="17"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3289,10 +3397,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="17"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3310,10 +3418,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="17"/>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3331,10 +3439,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="17"/>
+      <c r="J27" s="19"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3352,10 +3460,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="17"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3373,10 +3481,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="17"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3394,10 +3502,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="17"/>
+      <c r="J30" s="19"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3415,10 +3523,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="17"/>
+      <c r="J31" s="19"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3436,10 +3544,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="17"/>
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3457,10 +3565,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="17"/>
+      <c r="J33" s="19"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3478,10 +3586,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="17"/>
+      <c r="J34" s="19"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3499,10 +3607,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="17"/>
+      <c r="J35" s="19"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="4">
@@ -3522,7 +3630,7 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="4">
         <v>2</v>
       </c>
@@ -3540,7 +3648,7 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="4">
         <v>3</v>
       </c>
@@ -3558,7 +3666,7 @@
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="4">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
feat: update pinout table
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="131">
   <si>
     <t>Component</t>
   </si>
@@ -409,6 +409,27 @@
   </si>
   <si>
     <t>WIFI_EN</t>
+  </si>
+  <si>
+    <t>SCL_3V3</t>
+  </si>
+  <si>
+    <t>SDA_3V3</t>
+  </si>
+  <si>
+    <t>CAM_VSYNC</t>
+  </si>
+  <si>
+    <t>CAM_HREF</t>
+  </si>
+  <si>
+    <t>CAM_PCLK</t>
+  </si>
+  <si>
+    <t>CAM_XCLK</t>
+  </si>
+  <si>
+    <t>CAM_PWDN</t>
   </si>
 </sst>
 </file>
@@ -424,7 +445,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,12 +455,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -536,9 +551,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,10 +563,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -563,13 +575,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1431,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,52 +1462,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1505,158 +1517,158 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="19" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="18" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="10">
+      <c r="A5" s="17"/>
+      <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="19"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="10">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="19"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="10">
+      <c r="A7" s="17"/>
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="19"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="13" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="18"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="10">
+      <c r="A8" s="17"/>
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="19"/>
-      <c r="S8" s="21"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="18"/>
+      <c r="S8" s="20"/>
       <c r="T8" s="5" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="10">
+      <c r="A9" s="17"/>
+      <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9">
         <v>0</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="19"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="18"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="14" t="s">
+      <c r="T9" s="13" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5">
@@ -1678,27 +1690,27 @@
       <c r="I10" s="5">
         <v>3.6</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="S10" s="23"/>
-      <c r="T10" s="14" t="s">
+      <c r="S10" s="22"/>
+      <c r="T10" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1707,17 +1719,17 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="14" t="s">
+      <c r="J11" s="15"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1734,14 +1746,14 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1754,11 +1766,11 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="15"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1778,14 +1790,14 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1798,17 +1810,17 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>85</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1823,13 +1835,13 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="16"/>
+      <c r="J16" s="15"/>
       <c r="Q16" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1849,10 +1861,10 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="16"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5">
@@ -1861,7 +1873,7 @@
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1873,19 +1885,19 @@
       <c r="I18" s="5">
         <v>5</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1894,15 +1906,18 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="19"/>
+      <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>49</v>
@@ -1915,15 +1930,18 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="19"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>50</v>
@@ -1936,15 +1954,18 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="19"/>
+      <c r="J21" s="18"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>27</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>51</v>
@@ -1957,15 +1978,18 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>51</v>
@@ -1978,15 +2002,18 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="19"/>
+      <c r="J23" s="18"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>51</v>
@@ -1999,15 +2026,18 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>49</v>
@@ -2020,10 +2050,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="19"/>
+      <c r="J25" s="18"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
@@ -2044,10 +2074,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="19"/>
+      <c r="J26" s="18"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
@@ -2068,10 +2098,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="19"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
@@ -2092,10 +2122,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="19"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
@@ -2116,10 +2146,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="19"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
@@ -2140,10 +2170,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="19"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
@@ -2164,10 +2194,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="19"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
@@ -2188,10 +2218,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="19"/>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
@@ -2212,10 +2242,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="19"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2236,15 +2266,18 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="19"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>40</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>49</v>
@@ -2257,10 +2290,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="19"/>
+      <c r="J35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="5">
@@ -2269,7 +2302,7 @@
       <c r="C36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="8" t="s">
@@ -2280,19 +2313,19 @@
       <c r="H36" s="8">
         <v>0</v>
       </c>
-      <c r="J36" s="16" t="s">
+      <c r="J36" s="15" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="5">
         <v>2</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E37" s="8" t="s">
@@ -2303,17 +2336,17 @@
       <c r="H37" s="8">
         <v>5</v>
       </c>
-      <c r="J37" s="16"/>
+      <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="14"/>
       <c r="B38" s="5">
         <v>3</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="21" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="8" t="s">
@@ -2324,17 +2357,17 @@
       <c r="H38" s="8">
         <v>5</v>
       </c>
-      <c r="J38" s="16"/>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="5">
         <v>4</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="21" t="s">
         <v>90</v>
       </c>
       <c r="E39" s="8" t="s">
@@ -2345,10 +2378,10 @@
       <c r="H39" s="8">
         <v>5</v>
       </c>
-      <c r="J39" s="16"/>
+      <c r="J39" s="15"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2363,7 +2396,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2376,7 +2409,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2389,67 +2422,67 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2462,7 +2495,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2475,7 +2508,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2484,7 +2517,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2493,7 +2526,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2502,17 +2535,19 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="8"/>
+      <c r="D53" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2522,7 +2557,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2531,55 +2566,55 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D56" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>56</v>
+      <c r="D58" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="9" t="s">
-        <v>55</v>
+      <c r="D59" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2588,7 +2623,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2597,7 +2632,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2606,7 +2641,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2615,7 +2650,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2624,7 +2659,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
+      <c r="A65" s="15"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2633,31 +2668,31 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D66" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
+      <c r="A68" s="15"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2666,7 +2701,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2679,7 +2714,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2692,7 +2727,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2705,7 +2740,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2718,7 +2753,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2731,7 +2766,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2744,7 +2779,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2757,7 +2792,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2770,31 +2805,31 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="16"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="16"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
@@ -2807,7 +2842,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
@@ -2820,7 +2855,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="16"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2829,7 +2864,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2838,7 +2873,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="16"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2911,52 +2946,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -2966,10 +3001,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -2984,12 +3019,12 @@
       <c r="H4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -3002,10 +3037,10 @@
       <c r="H5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="19"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -3018,10 +3053,10 @@
       <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="19"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -3034,10 +3069,10 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="19"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -3056,10 +3091,10 @@
       <c r="I8" s="1">
         <v>5.5</v>
       </c>
-      <c r="J8" s="19"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3072,10 +3107,10 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="19"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -3094,12 +3129,12 @@
       <c r="I10" s="1">
         <v>3.6</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -3112,10 +3147,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="16"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3129,10 +3164,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3149,11 +3184,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="15"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3170,10 +3205,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3190,10 +3225,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3212,10 +3247,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="16"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3232,10 +3267,10 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="16"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1">
@@ -3253,12 +3288,12 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3271,10 +3306,10 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="19"/>
+      <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3292,10 +3327,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="19"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3313,10 +3348,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="19"/>
+      <c r="J21" s="18"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3334,10 +3369,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3355,10 +3390,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="19"/>
+      <c r="J23" s="18"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3376,10 +3411,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3397,10 +3432,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="19"/>
+      <c r="J25" s="18"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3418,10 +3453,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="19"/>
+      <c r="J26" s="18"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3439,10 +3474,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="19"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3460,10 +3495,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="19"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3481,10 +3516,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="19"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3502,10 +3537,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="19"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3523,10 +3558,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="19"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3544,10 +3579,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="19"/>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3565,10 +3600,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="19"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3586,10 +3621,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="19"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3607,10 +3642,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="19"/>
+      <c r="J35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="4">
@@ -3630,7 +3665,7 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="4">
         <v>2</v>
       </c>
@@ -3648,7 +3683,7 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="14"/>
       <c r="B38" s="4">
         <v>3</v>
       </c>
@@ -3666,7 +3701,7 @@
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="4">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
feat: add i2c ic, add additional datasheets and simulations
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolentino\Documents\test\Kicad\Projects\CameraSystem\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10590" windowHeight="8670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10590" windowHeight="8670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="5" r:id="rId1"/>
     <sheet name="Power Consumption" sheetId="3" r:id="rId2"/>
     <sheet name="Pinout_Old" sheetId="1" r:id="rId3"/>
+    <sheet name="Calculation" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="135">
   <si>
     <t>Component</t>
   </si>
@@ -431,12 +427,24 @@
   <si>
     <t>CAM_PWDN</t>
   </si>
+  <si>
+    <t>Oscillator Crystal</t>
+  </si>
+  <si>
+    <t>Cx</t>
+  </si>
+  <si>
+    <t>C_l</t>
+  </si>
+  <si>
+    <t>Cstray</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -557,11 +565,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -575,21 +595,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1433,21 +1442,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1461,53 +1470,53 @@
     <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:24">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+    <row r="3" spans="1:24">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1517,10 +1526,10 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="20" t="s">
         <v>104</v>
       </c>
       <c r="B4" s="9">
@@ -1541,12 +1550,12 @@
         <v>3.3</v>
       </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:24">
+      <c r="A5" s="21"/>
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -1565,10 +1574,10 @@
         <v>3.3</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="21"/>
       <c r="B6" s="9">
         <v>3</v>
       </c>
@@ -1587,10 +1596,10 @@
         <v>3.3</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" s="21"/>
       <c r="B7" s="9">
         <v>4</v>
       </c>
@@ -1609,14 +1618,14 @@
         <v>3.3</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="18"/>
+      <c r="J7" s="22"/>
       <c r="S7" s="10"/>
       <c r="T7" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:24">
+      <c r="A8" s="21"/>
       <c r="B8" s="9">
         <v>5</v>
       </c>
@@ -1635,14 +1644,14 @@
         <v>3.3</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="18"/>
-      <c r="S8" s="20"/>
+      <c r="J8" s="22"/>
+      <c r="S8" s="14"/>
       <c r="T8" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+    <row r="9" spans="1:24">
+      <c r="A9" s="21"/>
       <c r="B9" s="9">
         <v>6</v>
       </c>
@@ -1661,14 +1670,14 @@
         <v>0</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="18"/>
+      <c r="J9" s="22"/>
       <c r="S9" s="3"/>
       <c r="T9" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:24">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5">
@@ -1690,10 +1699,10 @@
       <c r="I10" s="5">
         <v>3.6</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="S10" s="22"/>
+      <c r="S10" s="16"/>
       <c r="T10" s="13" t="s">
         <v>121</v>
       </c>
@@ -1702,8 +1711,8 @@
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:24">
+      <c r="A11" s="18"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1719,8 +1728,8 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="S11" s="21"/>
+      <c r="J11" s="18"/>
+      <c r="S11" s="15"/>
       <c r="T11" s="13" t="s">
         <v>119</v>
       </c>
@@ -1728,8 +1737,8 @@
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+    <row r="12" spans="1:24">
+      <c r="A12" s="18"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1746,14 +1755,14 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="18"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1766,11 +1775,11 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="18"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+    <row r="14" spans="1:24">
+      <c r="A14" s="18"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1790,14 +1799,14 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" s="18"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1810,10 +1819,10 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="18"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1835,13 +1844,13 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="15"/>
+      <c r="J16" s="18"/>
       <c r="Q16" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+    <row r="17" spans="1:10">
+      <c r="A17" s="18"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1861,10 +1870,10 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5">
@@ -1885,12 +1894,12 @@
       <c r="I18" s="5">
         <v>5</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+    <row r="19" spans="1:10">
+      <c r="A19" s="18"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1906,10 +1915,10 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="18"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
@@ -1930,10 +1939,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="18"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
@@ -1954,10 +1963,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="18"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -1978,10 +1987,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="18"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -2002,10 +2011,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="18"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -2026,10 +2035,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="18"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="J24" s="22"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="18"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
@@ -2050,10 +2059,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="18"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="18"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
@@ -2074,10 +2083,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="18"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
@@ -2098,10 +2107,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="18"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
+      <c r="J27" s="22"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="18"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
@@ -2122,10 +2131,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="18"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="J28" s="22"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="18"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
@@ -2146,10 +2155,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="J29" s="22"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="18"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
@@ -2170,10 +2179,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="18"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="J30" s="22"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="18"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
@@ -2194,10 +2203,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="18"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="J31" s="22"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="18"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
@@ -2218,10 +2227,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="18"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="J32" s="22"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="18"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
@@ -2242,10 +2251,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="J33" s="22"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="18"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2266,10 +2275,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="J34" s="22"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="18"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
@@ -2290,10 +2299,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="J35" s="22"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" customHeight="1">
+      <c r="A36" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="5">
@@ -2313,12 +2322,12 @@
       <c r="H36" s="8">
         <v>0</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="J36" s="18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+    <row r="37" spans="1:10">
+      <c r="A37" s="19"/>
       <c r="B37" s="5">
         <v>2</v>
       </c>
@@ -2336,17 +2345,17 @@
       <c r="H37" s="8">
         <v>5</v>
       </c>
-      <c r="J37" s="15"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="J37" s="18"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="19"/>
       <c r="B38" s="5">
         <v>3</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="15" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="8" t="s">
@@ -2357,17 +2366,17 @@
       <c r="H38" s="8">
         <v>5</v>
       </c>
-      <c r="J38" s="15"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="J38" s="18"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="19"/>
       <c r="B39" s="5">
         <v>4</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="15" t="s">
         <v>90</v>
       </c>
       <c r="E39" s="8" t="s">
@@ -2378,10 +2387,10 @@
       <c r="H39" s="8">
         <v>5</v>
       </c>
-      <c r="J39" s="15"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="J39" s="18"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2395,8 +2404,8 @@
         <v>SD_MISO</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
+    <row r="41" spans="1:10">
+      <c r="A41" s="18"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2408,8 +2417,8 @@
         <v>SD_MOSI</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
+    <row r="42" spans="1:10">
+      <c r="A42" s="18"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2421,20 +2430,20 @@
         <v>SD_SCK</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
+    <row r="43" spans="1:10">
+      <c r="A43" s="18"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
+    <row r="44" spans="1:10">
+      <c r="A44" s="18"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
@@ -2445,8 +2454,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
+    <row r="45" spans="1:10">
+      <c r="A45" s="18"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
@@ -2457,32 +2466,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:10">
+      <c r="A46" s="18"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+    <row r="47" spans="1:10">
+      <c r="A47" s="18"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+    <row r="48" spans="1:10">
+      <c r="A48" s="18"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2494,8 +2503,8 @@
         <v>WIFI_TX</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
+    <row r="49" spans="1:4">
+      <c r="A49" s="18"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2507,8 +2516,8 @@
         <v>WIFI_RX</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+    <row r="50" spans="1:4">
+      <c r="A50" s="18"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2516,8 +2525,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
+    <row r="51" spans="1:4">
+      <c r="A51" s="18"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2525,8 +2534,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+    <row r="52" spans="1:4">
+      <c r="A52" s="18"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2534,8 +2543,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+    <row r="53" spans="1:4">
+      <c r="A53" s="18"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -2546,8 +2555,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+    <row r="54" spans="1:4">
+      <c r="A54" s="18"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2556,8 +2565,8 @@
       </c>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
+    <row r="55" spans="1:4">
+      <c r="A55" s="18"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2565,8 +2574,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+    <row r="56" spans="1:4">
+      <c r="A56" s="18"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
@@ -2577,8 +2586,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+    <row r="57" spans="1:4">
+      <c r="A57" s="18"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
@@ -2589,8 +2598,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+    <row r="58" spans="1:4">
+      <c r="A58" s="18"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
@@ -2601,8 +2610,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+    <row r="59" spans="1:4">
+      <c r="A59" s="18"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
@@ -2613,8 +2622,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+    <row r="60" spans="1:4">
+      <c r="A60" s="18"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2622,8 +2631,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:4">
+      <c r="A61" s="18"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2631,8 +2640,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+    <row r="62" spans="1:4">
+      <c r="A62" s="18"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2640,8 +2649,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
+    <row r="63" spans="1:4">
+      <c r="A63" s="18"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2649,8 +2658,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+    <row r="64" spans="1:4">
+      <c r="A64" s="18"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2658,8 +2667,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
+    <row r="65" spans="1:4">
+      <c r="A65" s="18"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2667,8 +2676,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
+    <row r="66" spans="1:4">
+      <c r="A66" s="18"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
@@ -2679,8 +2688,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
+    <row r="67" spans="1:4">
+      <c r="A67" s="18"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
@@ -2691,8 +2700,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
+    <row r="68" spans="1:4">
+      <c r="A68" s="18"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2700,8 +2709,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
+    <row r="69" spans="1:4">
+      <c r="A69" s="18"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2713,8 +2722,8 @@
         <v>CAM_D7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
+    <row r="70" spans="1:4">
+      <c r="A70" s="18"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2726,8 +2735,8 @@
         <v>CAM_D6</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
+    <row r="71" spans="1:4">
+      <c r="A71" s="18"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2739,8 +2748,8 @@
         <v>CAM_D5</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
+    <row r="72" spans="1:4">
+      <c r="A72" s="18"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2752,8 +2761,8 @@
         <v>CAM_D4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
+    <row r="73" spans="1:4">
+      <c r="A73" s="18"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2765,8 +2774,8 @@
         <v>CAM_D3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
+    <row r="74" spans="1:4">
+      <c r="A74" s="18"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2778,8 +2787,8 @@
         <v>CAM_D2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
+    <row r="75" spans="1:4">
+      <c r="A75" s="18"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2791,8 +2800,8 @@
         <v>CAM_D1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
+    <row r="76" spans="1:4">
+      <c r="A76" s="18"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2804,8 +2813,8 @@
         <v>CAM_D0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
+    <row r="77" spans="1:4">
+      <c r="A77" s="18"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
@@ -2816,8 +2825,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
+    <row r="78" spans="1:4">
+      <c r="A78" s="18"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
@@ -2828,8 +2837,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
+    <row r="79" spans="1:4">
+      <c r="A79" s="18"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
@@ -2841,8 +2850,8 @@
         <v>WIFI_EN</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
+    <row r="80" spans="1:4">
+      <c r="A80" s="18"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
@@ -2854,8 +2863,8 @@
         <v>WIFI_RST</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
+    <row r="81" spans="1:3">
+      <c r="A81" s="18"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2863,8 +2872,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="15"/>
+    <row r="82" spans="1:3">
+      <c r="A82" s="18"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2872,8 +2881,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
+    <row r="83" spans="1:3">
+      <c r="A83" s="18"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2886,14 +2895,6 @@
     <sortCondition descending="1" ref="H44"/>
   </sortState>
   <mergeCells count="18">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I2"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A83"/>
     <mergeCell ref="J2:J3"/>
@@ -2904,6 +2905,14 @@
     <mergeCell ref="A18:A35"/>
     <mergeCell ref="J18:J35"/>
     <mergeCell ref="J36:J39"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2912,26 +2921,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2945,53 +2954,53 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+    <row r="3" spans="1:12">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -3001,10 +3010,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -3019,12 +3028,12 @@
       <c r="H4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+    <row r="5" spans="1:12">
+      <c r="A5" s="18"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -3037,10 +3046,10 @@
       <c r="H5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="18"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -3053,10 +3062,10 @@
       <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="18"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -3069,10 +3078,10 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="18"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -3091,10 +3100,10 @@
       <c r="I8" s="1">
         <v>5.5</v>
       </c>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="18"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3107,10 +3116,10 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="J9" s="22"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -3129,12 +3138,12 @@
       <c r="I10" s="1">
         <v>3.6</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:12">
+      <c r="A11" s="18"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -3147,10 +3156,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="18"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3164,10 +3173,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="18"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3184,11 +3193,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="18"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+    <row r="14" spans="1:12">
+      <c r="A14" s="18"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3205,10 +3214,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="18"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3225,10 +3234,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="18"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3247,10 +3256,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="18"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3267,10 +3276,10 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1">
@@ -3288,12 +3297,12 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+    <row r="19" spans="1:10">
+      <c r="A19" s="18"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3306,10 +3315,10 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="18"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3327,10 +3336,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="18"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3348,10 +3357,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="18"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3369,10 +3378,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="18"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3390,10 +3399,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="18"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3411,10 +3420,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="18"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="J24" s="22"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="18"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3432,10 +3441,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="18"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="18"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3453,10 +3462,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="18"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3474,10 +3483,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="18"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
+      <c r="J27" s="22"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="18"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3495,10 +3504,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="18"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="J28" s="22"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="18"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3516,10 +3525,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="J29" s="22"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="18"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3537,10 +3546,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="18"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="J30" s="22"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="18"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3558,10 +3567,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="18"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="J31" s="22"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="18"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3579,10 +3588,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="18"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="J32" s="22"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="18"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3600,10 +3609,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="J33" s="22"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="18"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3621,10 +3630,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="J34" s="22"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="18"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3642,10 +3651,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="J35" s="22"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" customHeight="1">
+      <c r="A36" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="4">
@@ -3664,8 +3673,8 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+    <row r="37" spans="1:10">
+      <c r="A37" s="19"/>
       <c r="B37" s="4">
         <v>2</v>
       </c>
@@ -3682,8 +3691,8 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+    <row r="38" spans="1:10">
+      <c r="A38" s="19"/>
       <c r="B38" s="4">
         <v>3</v>
       </c>
@@ -3700,8 +3709,8 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+    <row r="39" spans="1:10">
+      <c r="A39" s="19"/>
       <c r="B39" s="4">
         <v>4</v>
       </c>
@@ -3718,7 +3727,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="7"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -3728,7 +3737,7 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="7"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -3760,4 +3769,49 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2">
+        <f>2*(B3-B4)</f>
+        <v>2.6000000000000001E-11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="24">
+        <v>1.7999999999999999E-11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="24">
+        <v>4.9999999999999997E-12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Camera System software first draft
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolentino\Documents\test\Kicad\Projects\CameraSystem\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10590" windowHeight="8670" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10590" windowHeight="8670" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="5" r:id="rId1"/>
     <sheet name="Power Consumption" sheetId="3" r:id="rId2"/>
     <sheet name="Pinout_Old" sheetId="1" r:id="rId3"/>
     <sheet name="Calculation" sheetId="6" r:id="rId4"/>
+    <sheet name="Changes" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="138">
   <si>
     <t>Component</t>
   </si>
@@ -439,12 +445,21 @@
   <si>
     <t>Cstray</t>
   </si>
+  <si>
+    <t>Connects LED to pin TXD (2) of CH340G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove 3 resistors (330Ohm) from SPI debug port </t>
+  </si>
+  <si>
+    <t>Remove pull-up resistor (10k Ohm) from CS line</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,11 +592,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -595,10 +611,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1442,21 +1457,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X83"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1470,35 +1485,35 @@
     <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="18" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="19" t="s">
@@ -1506,17 +1521,17 @@
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1526,10 +1541,10 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" s="20" t="s">
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>104</v>
       </c>
       <c r="B4" s="9">
@@ -1550,12 +1565,12 @@
         <v>3.3</v>
       </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
-      <c r="A5" s="21"/>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -1574,10 +1589,10 @@
         <v>3.3</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" s="21"/>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
       <c r="B6" s="9">
         <v>3</v>
       </c>
@@ -1596,10 +1611,10 @@
         <v>3.3</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" s="21"/>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
       <c r="B7" s="9">
         <v>4</v>
       </c>
@@ -1618,14 +1633,14 @@
         <v>3.3</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="22"/>
+      <c r="J7" s="23"/>
       <c r="S7" s="10"/>
       <c r="T7" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
-      <c r="A8" s="21"/>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
       <c r="B8" s="9">
         <v>5</v>
       </c>
@@ -1644,14 +1659,14 @@
         <v>3.3</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="22"/>
+      <c r="J8" s="23"/>
       <c r="S8" s="14"/>
       <c r="T8" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
-      <c r="A9" s="21"/>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
       <c r="B9" s="9">
         <v>6</v>
       </c>
@@ -1670,13 +1685,13 @@
         <v>0</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="22"/>
+      <c r="J9" s="23"/>
       <c r="S9" s="3"/>
       <c r="T9" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -1711,8 +1726,8 @@
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
     </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="18"/>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1728,7 +1743,7 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="18"/>
+      <c r="J11" s="20"/>
       <c r="S11" s="15"/>
       <c r="T11" s="13" t="s">
         <v>119</v>
@@ -1737,8 +1752,8 @@
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
     </row>
-    <row r="12" spans="1:24">
-      <c r="A12" s="18"/>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1755,10 +1770,10 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:24">
-      <c r="A13" s="18"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -1775,11 +1790,11 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="18"/>
+      <c r="J13" s="20"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:24">
-      <c r="A14" s="18"/>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1799,10 +1814,10 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:24">
-      <c r="A15" s="18"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -1819,10 +1834,10 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:24">
-      <c r="A16" s="18"/>
+      <c r="J15" s="20"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1844,13 +1859,13 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="18"/>
+      <c r="J16" s="20"/>
       <c r="Q16" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="18"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1870,9 +1885,9 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>7</v>
       </c>
@@ -1894,12 +1909,12 @@
       <c r="I18" s="5">
         <v>5</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1915,10 +1930,10 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="22"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="18"/>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
@@ -1939,10 +1954,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="22"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="18"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
@@ -1963,10 +1978,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="22"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="18"/>
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -1987,10 +2002,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="22"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="18"/>
+      <c r="J22" s="23"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -2011,10 +2026,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="22"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="18"/>
+      <c r="J23" s="23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -2035,10 +2050,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="22"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="18"/>
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
@@ -2059,10 +2074,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="22"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="18"/>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
@@ -2083,10 +2098,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="22"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="18"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
@@ -2107,10 +2122,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="22"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="18"/>
+      <c r="J27" s="23"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
@@ -2131,10 +2146,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="22"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="18"/>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
@@ -2155,10 +2170,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="22"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="18"/>
+      <c r="J29" s="23"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
@@ -2179,10 +2194,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="22"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="18"/>
+      <c r="J30" s="23"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
@@ -2203,10 +2218,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="22"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="18"/>
+      <c r="J31" s="23"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
@@ -2227,10 +2242,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="22"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="18"/>
+      <c r="J32" s="23"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
@@ -2251,10 +2266,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="22"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="18"/>
+      <c r="J33" s="23"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2275,10 +2290,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="22"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="18"/>
+      <c r="J34" s="23"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
@@ -2299,9 +2314,9 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="22"/>
-    </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1">
+      <c r="J35" s="23"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>54</v>
       </c>
@@ -2322,11 +2337,11 @@
       <c r="H36" s="8">
         <v>0</v>
       </c>
-      <c r="J36" s="18" t="s">
+      <c r="J36" s="20" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="5">
         <v>2</v>
@@ -2345,9 +2360,9 @@
       <c r="H37" s="8">
         <v>5</v>
       </c>
-      <c r="J37" s="18"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="5">
         <v>3</v>
@@ -2366,9 +2381,9 @@
       <c r="H38" s="8">
         <v>5</v>
       </c>
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="5">
         <v>4</v>
@@ -2387,10 +2402,10 @@
       <c r="H39" s="8">
         <v>5</v>
       </c>
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="18" t="s">
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2404,8 +2419,8 @@
         <v>SD_MISO</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="18"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2417,8 +2432,8 @@
         <v>SD_MOSI</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="18"/>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2430,8 +2445,8 @@
         <v>SD_SCK</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="18"/>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
@@ -2442,8 +2457,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="18"/>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
@@ -2454,8 +2469,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="18"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="20"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
@@ -2466,8 +2481,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="18"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="20"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
@@ -2478,8 +2493,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="18"/>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
@@ -2490,8 +2505,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="18"/>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2503,8 +2518,8 @@
         <v>WIFI_TX</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="18"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2516,8 +2531,8 @@
         <v>WIFI_RX</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="18"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2525,8 +2540,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="18"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2534,8 +2549,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="18"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2543,8 +2558,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="18"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -2555,8 +2570,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="18"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2565,8 +2580,8 @@
       </c>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="18"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="20"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2574,8 +2589,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="18"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
@@ -2586,8 +2601,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="18"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="20"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
@@ -2598,8 +2613,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="18"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="20"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
@@ -2610,8 +2625,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="18"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="20"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
@@ -2622,8 +2637,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="18"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="20"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2631,8 +2646,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="18"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2640,8 +2655,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="18"/>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="20"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2649,8 +2664,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="18"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="20"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2658,8 +2673,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="18"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="20"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2667,8 +2682,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="18"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="20"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2676,8 +2691,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="18"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="20"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
@@ -2688,8 +2703,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="18"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
@@ -2700,8 +2715,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="18"/>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="20"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2709,8 +2724,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="18"/>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="20"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2722,8 +2737,8 @@
         <v>CAM_D7</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="18"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="20"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2735,8 +2750,8 @@
         <v>CAM_D6</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="18"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="20"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2748,8 +2763,8 @@
         <v>CAM_D5</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="18"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2761,8 +2776,8 @@
         <v>CAM_D4</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="18"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="20"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2774,8 +2789,8 @@
         <v>CAM_D3</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="18"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="20"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2787,8 +2802,8 @@
         <v>CAM_D2</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="18"/>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="20"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2800,8 +2815,8 @@
         <v>CAM_D1</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="18"/>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="20"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2813,8 +2828,8 @@
         <v>CAM_D0</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="18"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="20"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
@@ -2825,8 +2840,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="18"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="20"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
@@ -2837,8 +2852,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="18"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="20"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
@@ -2850,8 +2865,8 @@
         <v>WIFI_EN</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="18"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="20"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
@@ -2863,8 +2878,8 @@
         <v>WIFI_RST</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="18"/>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="20"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2872,8 +2887,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="18"/>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="20"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2881,8 +2896,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="18"/>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="20"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2895,6 +2910,14 @@
     <sortCondition descending="1" ref="H44"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A83"/>
     <mergeCell ref="J2:J3"/>
@@ -2905,14 +2928,6 @@
     <mergeCell ref="A18:A35"/>
     <mergeCell ref="J18:J35"/>
     <mergeCell ref="J36:J39"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2921,26 +2936,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2954,35 +2969,35 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="18" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="19" t="s">
@@ -2990,17 +3005,17 @@
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -3010,10 +3025,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="18" t="s">
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -3028,12 +3043,12 @@
       <c r="H4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="18"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -3046,10 +3061,10 @@
       <c r="H5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="18"/>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -3062,10 +3077,10 @@
       <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="18"/>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -3078,10 +3093,10 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="22"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="18"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -3100,10 +3115,10 @@
       <c r="I8" s="1">
         <v>5.5</v>
       </c>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="18"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3116,9 +3131,9 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="22"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
@@ -3142,8 +3157,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="18"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -3156,10 +3171,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="18"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3173,10 +3188,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="18"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3193,11 +3208,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="18"/>
+      <c r="J13" s="20"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="18"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3214,10 +3229,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="18"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3234,10 +3249,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="18"/>
+      <c r="J15" s="20"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3256,10 +3271,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="18"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3276,9 +3291,9 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>7</v>
       </c>
@@ -3297,12 +3312,12 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3315,10 +3330,10 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="22"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="18"/>
+      <c r="J19" s="23"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3336,10 +3351,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="22"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="18"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3357,10 +3372,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="22"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="18"/>
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3378,10 +3393,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="22"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="18"/>
+      <c r="J22" s="23"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3399,10 +3414,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="22"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="18"/>
+      <c r="J23" s="23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3420,10 +3435,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="22"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="18"/>
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3441,10 +3456,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="22"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="18"/>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3462,10 +3477,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="22"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="18"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3483,10 +3498,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="22"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="18"/>
+      <c r="J27" s="23"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3504,10 +3519,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="22"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="18"/>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3525,10 +3540,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="22"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="18"/>
+      <c r="J29" s="23"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3546,10 +3561,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="22"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="18"/>
+      <c r="J30" s="23"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3567,10 +3582,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="22"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="18"/>
+      <c r="J31" s="23"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3588,10 +3603,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="22"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="18"/>
+      <c r="J32" s="23"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3609,10 +3624,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="22"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="18"/>
+      <c r="J33" s="23"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3630,10 +3645,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="22"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="18"/>
+      <c r="J34" s="23"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3651,9 +3666,9 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="22"/>
-    </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1">
+      <c r="J35" s="23"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>54</v>
       </c>
@@ -3673,7 +3688,7 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="4">
         <v>2</v>
@@ -3691,7 +3706,7 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="19"/>
       <c r="B38" s="4">
         <v>3</v>
@@ -3709,7 +3724,7 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="4">
         <v>4</v>
@@ -3727,7 +3742,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -3737,7 +3752,7 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -3772,21 +3787,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -3795,23 +3810,53 @@
         <v>2.6000000000000001E-11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="18">
         <v>1.7999999999999999E-11</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="18">
         <v>4.9999999999999997E-12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Camera System QT Pad schematic reviewed
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="143">
   <si>
     <t>Component</t>
   </si>
@@ -452,7 +452,22 @@
     <t xml:space="preserve">Remove 3 resistors (330Ohm) from SPI debug port </t>
   </si>
   <si>
-    <t>Remove pull-up resistor (10k Ohm) from CS line</t>
+    <t>Remove pull-up resistor (10k Ohm) from CS line - Memory</t>
+  </si>
+  <si>
+    <t>Resistor kept but notation to active low added</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Assign QT pins</t>
   </si>
 </sst>
 </file>
@@ -594,10 +609,10 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1486,52 +1501,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1541,7 +1556,7 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="20"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -1692,7 +1707,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5">
@@ -1714,7 +1729,7 @@
       <c r="I10" s="5">
         <v>3.6</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="20" t="s">
         <v>53</v>
       </c>
       <c r="S10" s="16"/>
@@ -1727,7 +1742,7 @@
       <c r="X10" s="12"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1743,7 +1758,7 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="20"/>
+      <c r="J11" s="19"/>
       <c r="S11" s="15"/>
       <c r="T11" s="13" t="s">
         <v>119</v>
@@ -1753,7 +1768,7 @@
       <c r="W11" s="12"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1770,10 +1785,10 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="20"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -1790,11 +1805,11 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="20"/>
+      <c r="J13" s="19"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1814,10 +1829,10 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="20"/>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -1834,10 +1849,10 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="20"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1859,13 +1874,13 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="20"/>
+      <c r="J16" s="19"/>
       <c r="Q16" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1885,10 +1900,10 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="20"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5">
@@ -1914,7 +1929,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1933,7 +1948,7 @@
       <c r="J19" s="23"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
@@ -1957,7 +1972,7 @@
       <c r="J20" s="23"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
@@ -1981,7 +1996,7 @@
       <c r="J21" s="23"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -2005,7 +2020,7 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -2029,7 +2044,7 @@
       <c r="J23" s="23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -2053,7 +2068,7 @@
       <c r="J24" s="23"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
@@ -2077,7 +2092,7 @@
       <c r="J25" s="23"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
@@ -2101,7 +2116,7 @@
       <c r="J26" s="23"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
@@ -2125,7 +2140,7 @@
       <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
@@ -2149,7 +2164,7 @@
       <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
@@ -2173,7 +2188,7 @@
       <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
@@ -2197,7 +2212,7 @@
       <c r="J30" s="23"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
@@ -2221,7 +2236,7 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
@@ -2245,7 +2260,7 @@
       <c r="J32" s="23"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
@@ -2269,7 +2284,7 @@
       <c r="J33" s="23"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2293,7 +2308,7 @@
       <c r="J34" s="23"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
@@ -2317,7 +2332,7 @@
       <c r="J35" s="23"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="5">
@@ -2337,12 +2352,12 @@
       <c r="H36" s="8">
         <v>0</v>
       </c>
-      <c r="J36" s="20" t="s">
+      <c r="J36" s="19" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="5">
         <v>2</v>
       </c>
@@ -2360,10 +2375,10 @@
       <c r="H37" s="8">
         <v>5</v>
       </c>
-      <c r="J37" s="20"/>
+      <c r="J37" s="19"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="5">
         <v>3</v>
       </c>
@@ -2381,10 +2396,10 @@
       <c r="H38" s="8">
         <v>5</v>
       </c>
-      <c r="J38" s="20"/>
+      <c r="J38" s="19"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="5">
         <v>4</v>
       </c>
@@ -2402,10 +2417,10 @@
       <c r="H39" s="8">
         <v>5</v>
       </c>
-      <c r="J39" s="20"/>
+      <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2420,7 +2435,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2433,7 +2448,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2446,7 +2461,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
@@ -2458,7 +2473,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
@@ -2470,7 +2485,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
@@ -2482,7 +2497,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
@@ -2494,7 +2509,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
@@ -2506,7 +2521,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2519,7 +2534,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2532,7 +2547,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2541,7 +2556,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2550,7 +2565,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2559,7 +2574,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -2571,7 +2586,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2581,7 +2596,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2590,7 +2605,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
@@ -2602,7 +2617,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
@@ -2614,7 +2629,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
@@ -2626,7 +2641,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
@@ -2638,7 +2653,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2647,7 +2662,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2656,7 +2671,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2665,7 +2680,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2674,7 +2689,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2683,7 +2698,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2692,7 +2707,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
+      <c r="A66" s="19"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
@@ -2704,7 +2719,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
@@ -2716,7 +2731,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2725,7 +2740,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2738,7 +2753,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2751,7 +2766,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2764,7 +2779,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2777,7 +2792,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2790,7 +2805,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="20"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2803,7 +2818,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="20"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2816,7 +2831,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="20"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2829,7 +2844,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="20"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
@@ -2841,7 +2856,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="20"/>
+      <c r="A78" s="19"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
@@ -2853,7 +2868,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="20"/>
+      <c r="A79" s="19"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
@@ -2866,7 +2881,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="20"/>
+      <c r="A80" s="19"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
@@ -2879,7 +2894,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="20"/>
+      <c r="A81" s="19"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2888,7 +2903,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
+      <c r="A82" s="19"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2897,7 +2912,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
+      <c r="A83" s="19"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2910,14 +2925,6 @@
     <sortCondition descending="1" ref="H44"/>
   </sortState>
   <mergeCells count="18">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I2"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A83"/>
     <mergeCell ref="J2:J3"/>
@@ -2928,6 +2935,14 @@
     <mergeCell ref="A18:A35"/>
     <mergeCell ref="J18:J35"/>
     <mergeCell ref="J36:J39"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2970,52 +2985,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -3025,10 +3040,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="20"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -3048,7 +3063,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -3064,7 +3079,7 @@
       <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -3080,7 +3095,7 @@
       <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -3096,7 +3111,7 @@
       <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -3118,7 +3133,7 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3134,7 +3149,7 @@
       <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -3153,12 +3168,12 @@
       <c r="I10" s="1">
         <v>3.6</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -3171,10 +3186,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="20"/>
+      <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3188,10 +3203,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="20"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3208,11 +3223,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="20"/>
+      <c r="J13" s="19"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3229,10 +3244,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="20"/>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3249,10 +3264,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="20"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3271,10 +3286,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="20"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3291,10 +3306,10 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="20"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1">
@@ -3317,7 +3332,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3333,7 +3348,7 @@
       <c r="J19" s="23"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3354,7 +3369,7 @@
       <c r="J20" s="23"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3375,7 +3390,7 @@
       <c r="J21" s="23"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3396,7 +3411,7 @@
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3417,7 +3432,7 @@
       <c r="J23" s="23"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3438,7 +3453,7 @@
       <c r="J24" s="23"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3459,7 +3474,7 @@
       <c r="J25" s="23"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3480,7 +3495,7 @@
       <c r="J26" s="23"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3501,7 +3516,7 @@
       <c r="J27" s="23"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3522,7 +3537,7 @@
       <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3543,7 +3558,7 @@
       <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3564,7 +3579,7 @@
       <c r="J30" s="23"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3585,7 +3600,7 @@
       <c r="J31" s="23"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3606,7 +3621,7 @@
       <c r="J32" s="23"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3627,7 +3642,7 @@
       <c r="J33" s="23"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3648,7 +3663,7 @@
       <c r="J34" s="23"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3669,7 +3684,7 @@
       <c r="J35" s="23"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="4">
@@ -3689,7 +3704,7 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="4">
         <v>2</v>
       </c>
@@ -3707,7 +3722,7 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="4">
         <v>3</v>
       </c>
@@ -3725,7 +3740,7 @@
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="4">
         <v>4</v>
       </c>
@@ -3833,27 +3848,53 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replace tvs diodes of camera system
</commit_message>
<xml_diff>
--- a/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
+++ b/Projects/CameraSystem/Docs/CameraSystemSpecs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolentino\Documents\test\Kicad\Projects\CameraSystem\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolentino\Documents\Kicad\Projects\CameraSystem\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="148">
   <si>
     <t>Component</t>
   </si>
@@ -468,6 +468,21 @@
   </si>
   <si>
     <t>Assign QT pins</t>
+  </si>
+  <si>
+    <t>Swap Serial -&gt; MOSI to MOSI and MISO to MISO</t>
+  </si>
+  <si>
+    <t>Remove C10 so that C6 can be used for the autoreset</t>
+  </si>
+  <si>
+    <t>Replace D1 with plus tvs diodes</t>
+  </si>
+  <si>
+    <t>Replace D5 Zener with TVS Diode (Diode removed)</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -483,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +547,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -554,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,11 +629,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -625,6 +649,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1501,34 +1529,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="20" t="s">
@@ -1536,17 +1564,17 @@
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1556,10 +1584,10 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="19"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>104</v>
       </c>
       <c r="B4" s="9">
@@ -1580,12 +1608,12 @@
         <v>3.3</v>
       </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="24" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -1604,10 +1632,10 @@
         <v>3.3</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="23"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="9">
         <v>3</v>
       </c>
@@ -1626,10 +1654,10 @@
         <v>3.3</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="23"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="9">
         <v>4</v>
       </c>
@@ -1648,14 +1676,14 @@
         <v>3.3</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="23"/>
+      <c r="J7" s="24"/>
       <c r="S7" s="10"/>
       <c r="T7" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="9">
         <v>5</v>
       </c>
@@ -1674,14 +1702,14 @@
         <v>3.3</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="23"/>
+      <c r="J8" s="24"/>
       <c r="S8" s="14"/>
       <c r="T8" s="5" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="9">
         <v>6</v>
       </c>
@@ -1700,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="24"/>
       <c r="S9" s="3"/>
       <c r="T9" s="13" t="s">
         <v>120</v>
@@ -1742,7 +1770,7 @@
       <c r="X10" s="12"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -1758,7 +1786,7 @@
       <c r="H11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="19"/>
+      <c r="J11" s="21"/>
       <c r="S11" s="15"/>
       <c r="T11" s="13" t="s">
         <v>119</v>
@@ -1768,7 +1796,7 @@
       <c r="W11" s="12"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -1785,10 +1813,10 @@
       <c r="I12" s="5">
         <v>3.6</v>
       </c>
-      <c r="J12" s="19"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -1805,11 +1833,11 @@
       <c r="I13" s="5">
         <v>3.6</v>
       </c>
-      <c r="J13" s="19"/>
+      <c r="J13" s="21"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -1829,10 +1857,10 @@
       <c r="I14" s="5">
         <v>3.6</v>
       </c>
-      <c r="J14" s="19"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -1849,10 +1877,10 @@
       <c r="I15" s="5">
         <v>3.6</v>
       </c>
-      <c r="J15" s="19"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1874,13 +1902,13 @@
       <c r="I16" s="5">
         <v>3.6</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="21"/>
       <c r="Q16" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -1900,7 +1928,7 @@
       <c r="I17" s="5">
         <v>3.6</v>
       </c>
-      <c r="J17" s="19"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
@@ -1924,12 +1952,12 @@
       <c r="I18" s="5">
         <v>5</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="5">
         <v>2</v>
       </c>
@@ -1945,10 +1973,10 @@
       <c r="H19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="23"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="5">
         <v>3</v>
       </c>
@@ -1969,10 +1997,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="23"/>
+      <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="5">
         <v>4</v>
       </c>
@@ -1993,10 +2021,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="23"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5">
         <v>5</v>
       </c>
@@ -2017,10 +2045,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="5">
         <v>6</v>
       </c>
@@ -2041,10 +2069,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="23"/>
+      <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -2065,10 +2093,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="23"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="5">
         <v>8</v>
       </c>
@@ -2089,10 +2117,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="23"/>
+      <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="5">
         <v>9</v>
       </c>
@@ -2113,10 +2141,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="23"/>
+      <c r="J26" s="24"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5">
         <v>10</v>
       </c>
@@ -2137,10 +2165,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="23"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5">
         <v>11</v>
       </c>
@@ -2161,10 +2189,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="23"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5">
         <v>12</v>
       </c>
@@ -2185,10 +2213,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="23"/>
+      <c r="J29" s="24"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5">
         <v>13</v>
       </c>
@@ -2209,10 +2237,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="23"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="5">
         <v>14</v>
       </c>
@@ -2233,10 +2261,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="23"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="5">
         <v>15</v>
       </c>
@@ -2257,10 +2285,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="23"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="5">
         <v>16</v>
       </c>
@@ -2281,10 +2309,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="23"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="5">
         <v>17</v>
       </c>
@@ -2305,10 +2333,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="23"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="5">
         <v>18</v>
       </c>
@@ -2329,7 +2357,7 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="23"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
@@ -2352,7 +2380,7 @@
       <c r="H36" s="8">
         <v>0</v>
       </c>
-      <c r="J36" s="19" t="s">
+      <c r="J36" s="21" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2375,7 +2403,7 @@
       <c r="H37" s="8">
         <v>5</v>
       </c>
-      <c r="J37" s="19"/>
+      <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
@@ -2396,7 +2424,7 @@
       <c r="H38" s="8">
         <v>5</v>
       </c>
-      <c r="J38" s="19"/>
+      <c r="J38" s="21"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
@@ -2417,10 +2445,10 @@
       <c r="H39" s="8">
         <v>5</v>
       </c>
-      <c r="J39" s="19"/>
+      <c r="J39" s="21"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="21" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="5">
@@ -2435,7 +2463,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="5">
         <v>2</v>
       </c>
@@ -2448,7 +2476,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="5">
         <v>3</v>
       </c>
@@ -2461,7 +2489,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="5">
         <v>4</v>
       </c>
@@ -2473,7 +2501,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="5">
         <v>5</v>
       </c>
@@ -2485,7 +2513,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="5">
         <v>6</v>
       </c>
@@ -2497,7 +2525,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="5">
         <v>7</v>
       </c>
@@ -2509,7 +2537,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="5">
         <v>8</v>
       </c>
@@ -2521,7 +2549,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="5">
         <v>9</v>
       </c>
@@ -2534,7 +2562,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="5">
         <v>10</v>
       </c>
@@ -2547,7 +2575,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="5">
         <v>11</v>
       </c>
@@ -2556,7 +2584,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="5">
         <v>12</v>
       </c>
@@ -2565,7 +2593,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="5">
         <v>13</v>
       </c>
@@ -2574,7 +2602,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="5">
         <v>14</v>
       </c>
@@ -2586,7 +2614,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="5">
         <v>15</v>
       </c>
@@ -2596,7 +2624,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="5">
         <v>16</v>
       </c>
@@ -2605,7 +2633,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="5">
         <v>17</v>
       </c>
@@ -2617,7 +2645,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="5">
         <v>18</v>
       </c>
@@ -2629,7 +2657,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="5">
         <v>19</v>
       </c>
@@ -2641,7 +2669,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="5">
         <v>20</v>
       </c>
@@ -2653,7 +2681,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="5">
         <v>21</v>
       </c>
@@ -2662,7 +2690,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="5">
         <v>22</v>
       </c>
@@ -2671,7 +2699,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="5">
         <v>23</v>
       </c>
@@ -2680,7 +2708,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="5">
         <v>24</v>
       </c>
@@ -2689,7 +2717,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="19"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="5">
         <v>25</v>
       </c>
@@ -2698,7 +2726,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="5">
         <v>26</v>
       </c>
@@ -2707,7 +2735,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="19"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5">
         <v>27</v>
       </c>
@@ -2719,7 +2747,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="5">
         <v>28</v>
       </c>
@@ -2731,7 +2759,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="5">
         <v>29</v>
       </c>
@@ -2740,7 +2768,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
+      <c r="A69" s="21"/>
       <c r="B69" s="5">
         <v>30</v>
       </c>
@@ -2753,7 +2781,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="5">
         <v>31</v>
       </c>
@@ -2766,7 +2794,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="5">
         <v>32</v>
       </c>
@@ -2779,7 +2807,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="5">
         <v>33</v>
       </c>
@@ -2792,7 +2820,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="19"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="5">
         <v>34</v>
       </c>
@@ -2805,7 +2833,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="19"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="5">
         <v>35</v>
       </c>
@@ -2818,7 +2846,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="19"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="5">
         <v>36</v>
       </c>
@@ -2831,7 +2859,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="19"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="5">
         <v>37</v>
       </c>
@@ -2844,7 +2872,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="19"/>
+      <c r="A77" s="21"/>
       <c r="B77" s="5">
         <v>38</v>
       </c>
@@ -2856,7 +2884,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="19"/>
+      <c r="A78" s="21"/>
       <c r="B78" s="5">
         <v>39</v>
       </c>
@@ -2868,7 +2896,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="19"/>
+      <c r="A79" s="21"/>
       <c r="B79" s="5">
         <v>40</v>
       </c>
@@ -2881,7 +2909,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="5">
         <v>41</v>
       </c>
@@ -2894,7 +2922,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="19"/>
+      <c r="A81" s="21"/>
       <c r="B81" s="5">
         <v>42</v>
       </c>
@@ -2903,7 +2931,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="19"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="5">
         <v>43</v>
       </c>
@@ -2912,7 +2940,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="19"/>
+      <c r="A83" s="21"/>
       <c r="B83" s="5">
         <v>44</v>
       </c>
@@ -2925,6 +2953,14 @@
     <sortCondition descending="1" ref="H44"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A40:A83"/>
     <mergeCell ref="J2:J3"/>
@@ -2935,14 +2971,6 @@
     <mergeCell ref="A18:A35"/>
     <mergeCell ref="J18:J35"/>
     <mergeCell ref="J36:J39"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2985,34 +3013,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="20" t="s">
@@ -3020,17 +3048,17 @@
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
@@ -3040,10 +3068,10 @@
       <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="19"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -3058,12 +3086,12 @@
       <c r="H4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="24" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -3076,10 +3104,10 @@
       <c r="H5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="23"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -3092,10 +3120,10 @@
       <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="23"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -3108,10 +3136,10 @@
       <c r="H7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="23"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -3130,10 +3158,10 @@
       <c r="I8" s="1">
         <v>5.5</v>
       </c>
-      <c r="J8" s="23"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3146,7 +3174,7 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="23"/>
+      <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -3173,7 +3201,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -3186,10 +3214,10 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="19"/>
+      <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3203,10 +3231,10 @@
       <c r="I12" s="1">
         <v>3.6</v>
       </c>
-      <c r="J12" s="19"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -3223,11 +3251,11 @@
       <c r="I13" s="1">
         <v>3.6</v>
       </c>
-      <c r="J13" s="19"/>
+      <c r="J13" s="21"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="1">
         <v>5</v>
       </c>
@@ -3244,10 +3272,10 @@
       <c r="I14" s="1">
         <v>3.6</v>
       </c>
-      <c r="J14" s="19"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -3264,10 +3292,10 @@
       <c r="I15" s="1">
         <v>3.6</v>
       </c>
-      <c r="J15" s="19"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -3286,10 +3314,10 @@
       <c r="I16" s="1">
         <v>3.6</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -3306,7 +3334,7 @@
       <c r="I17" s="1">
         <v>3.6</v>
       </c>
-      <c r="J17" s="19"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
@@ -3327,12 +3355,12 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -3345,10 +3373,10 @@
       <c r="H19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="23"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -3366,10 +3394,10 @@
         <f t="shared" ref="I20:I35" si="0">2.8+0.5</f>
         <v>3.3</v>
       </c>
-      <c r="J20" s="23"/>
+      <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="1">
         <v>4</v>
       </c>
@@ -3387,10 +3415,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J21" s="23"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="1">
         <v>5</v>
       </c>
@@ -3408,10 +3436,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="1">
         <v>6</v>
       </c>
@@ -3429,10 +3457,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J23" s="23"/>
+      <c r="J23" s="24"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="1">
         <v>7</v>
       </c>
@@ -3450,10 +3478,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J24" s="23"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="1">
         <v>8</v>
       </c>
@@ -3471,10 +3499,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J25" s="23"/>
+      <c r="J25" s="24"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -3492,10 +3520,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J26" s="23"/>
+      <c r="J26" s="24"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="1">
         <v>10</v>
       </c>
@@ -3513,10 +3541,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J27" s="23"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -3534,10 +3562,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J28" s="23"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="1">
         <v>12</v>
       </c>
@@ -3555,10 +3583,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J29" s="23"/>
+      <c r="J29" s="24"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="1">
         <v>13</v>
       </c>
@@ -3576,10 +3604,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J30" s="23"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="1">
         <v>14</v>
       </c>
@@ -3597,10 +3625,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J31" s="23"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="1">
         <v>15</v>
       </c>
@@ -3618,10 +3646,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J32" s="23"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="1">
         <v>16</v>
       </c>
@@ -3639,10 +3667,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J33" s="23"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="1">
         <v>17</v>
       </c>
@@ -3660,10 +3688,10 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J34" s="23"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="1">
         <v>18</v>
       </c>
@@ -3681,7 +3709,7 @@
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J35" s="23"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
@@ -3848,10 +3876,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3860,42 +3888,86 @@
     <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="27" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" s="27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="26"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" s="26"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="19" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" s="26"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>142</v>
       </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="26"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="26"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="26"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>